<commit_message>
LCA in a BST
</commit_message>
<xml_diff>
--- a/DSA-450/FINAL450.xlsx
+++ b/DSA-450/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\DSA\DSA-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB516B57-2705-4655-A588-DF6319A4F08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421D2514-6F30-41B6-A800-23AF13256842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1999,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="B1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>

</xml_diff>